<commit_message>
modif du fichier mapping
</commit_message>
<xml_diff>
--- a/Data Hospital/Hopital Mapping VF.xlsx
+++ b/Data Hospital/Hopital Mapping VF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P997156\Documents\00. ST\NF26\01.inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\Documents\ETUDE\UTC semestre 4\NF26\Smart-Teem\nf26_smart_teem\Data Hospital\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35F9DE4-9859-43FA-9938-A3E9BCA6C6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87A5197-33BC-40EE-B316-4FD7551E30C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{783B3F39-6BFD-C940-8606-2E6B97310E4C}"/>
+    <workbookView xWindow="14400" yWindow="-16200" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{783B3F39-6BFD-C940-8606-2E6B97310E4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Staging" sheetId="1" r:id="rId1"/>
@@ -21,15 +21,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -996,7 +987,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1025,7 +1016,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1053,6 +1044,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF204E78"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1159,7 +1156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1209,6 +1206,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1554,27 +1552,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{769CA4DD-88B4-584F-8493-2F25A9DD02C6}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.84375" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.84375" style="1"/>
-    <col min="6" max="6" width="25.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.4609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.84375" style="1"/>
-    <col min="10" max="10" width="48.69140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.84375" style="1"/>
+    <col min="5" max="5" width="10.796875" style="1"/>
+    <col min="6" max="6" width="25.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.796875" style="1"/>
+    <col min="10" max="10" width="48.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>137</v>
       </c>
@@ -1590,7 +1588,7 @@
       <c r="I1" s="22"/>
       <c r="J1" s="23"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>134</v>
       </c>
@@ -1622,7 +1620,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1654,7 +1652,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1686,7 +1684,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1714,7 +1712,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1742,7 +1740,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1770,7 +1768,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -1802,7 +1800,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1834,7 +1832,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1866,7 +1864,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
@@ -1898,7 +1896,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
@@ -1930,7 +1928,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
@@ -1962,7 +1960,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
@@ -1990,7 +1988,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
@@ -2022,7 +2020,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>8</v>
       </c>
@@ -2054,7 +2052,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
@@ -2086,7 +2084,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -2118,7 +2116,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -2150,7 +2148,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>13</v>
       </c>
@@ -2182,7 +2180,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>13</v>
       </c>
@@ -2214,7 +2212,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
@@ -2246,7 +2244,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>13</v>
       </c>
@@ -2274,7 +2272,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>13</v>
       </c>
@@ -2302,7 +2300,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
@@ -2334,7 +2332,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>13</v>
       </c>
@@ -2366,7 +2364,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>13</v>
       </c>
@@ -2398,7 +2396,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>23</v>
       </c>
@@ -2430,7 +2428,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>23</v>
       </c>
@@ -2462,7 +2460,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>23</v>
       </c>
@@ -2494,7 +2492,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>23</v>
       </c>
@@ -2522,7 +2520,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>23</v>
       </c>
@@ -2550,7 +2548,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>23</v>
       </c>
@@ -2578,7 +2576,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>23</v>
       </c>
@@ -2606,7 +2604,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>23</v>
       </c>
@@ -2634,7 +2632,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>23</v>
       </c>
@@ -2662,7 +2660,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>23</v>
       </c>
@@ -2690,7 +2688,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>23</v>
       </c>
@@ -2718,7 +2716,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>23</v>
       </c>
@@ -2746,7 +2744,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>23</v>
       </c>
@@ -2774,7 +2772,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>23</v>
       </c>
@@ -2802,7 +2800,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>23</v>
       </c>
@@ -2830,7 +2828,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>23</v>
       </c>
@@ -2862,7 +2860,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>23</v>
       </c>
@@ -2894,7 +2892,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>40</v>
       </c>
@@ -2926,7 +2924,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>40</v>
       </c>
@@ -2958,7 +2956,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>40</v>
       </c>
@@ -2990,7 +2988,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>40</v>
       </c>
@@ -3022,7 +3020,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>40</v>
       </c>
@@ -3054,7 +3052,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>40</v>
       </c>
@@ -3086,7 +3084,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>40</v>
       </c>
@@ -3114,7 +3112,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>40</v>
       </c>
@@ -3142,7 +3140,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>40</v>
       </c>
@@ -3170,7 +3168,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>40</v>
       </c>
@@ -3198,7 +3196,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>40</v>
       </c>
@@ -3226,7 +3224,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>40</v>
       </c>
@@ -3254,7 +3252,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>40</v>
       </c>
@@ -3282,7 +3280,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>58</v>
       </c>
@@ -3314,7 +3312,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>58</v>
       </c>
@@ -3346,7 +3344,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>58</v>
       </c>
@@ -3378,7 +3376,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>58</v>
       </c>
@@ -3410,7 +3408,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>58</v>
       </c>
@@ -3438,7 +3436,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>58</v>
       </c>
@@ -3466,7 +3464,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>58</v>
       </c>
@@ -3498,7 +3496,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>57</v>
       </c>
@@ -3530,7 +3528,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>57</v>
       </c>
@@ -3558,7 +3556,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>57</v>
       </c>
@@ -3586,7 +3584,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>57</v>
       </c>
@@ -3618,7 +3616,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>57</v>
       </c>
@@ -3662,29 +3660,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAFCA74-9FC5-C241-99E0-C2C69841C5BE}">
-  <dimension ref="A1:O101"/>
+  <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.09765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.15234375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.15234375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.4609375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="47.15234375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="49.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="47.09765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="49.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>137</v>
       </c>
@@ -3705,7 +3703,7 @@
       <c r="N1" s="25"/>
       <c r="O1" s="26"/>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>141</v>
       </c>
@@ -3752,7 +3750,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>146</v>
       </c>
@@ -3798,8 +3796,9 @@
       <c r="O3" s="13" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3" s="27"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>146</v>
       </c>
@@ -3841,8 +3840,9 @@
       <c r="O4" s="13" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4" s="27"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>146</v>
       </c>
@@ -3880,8 +3880,9 @@
       <c r="O5" s="13" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5" s="27"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>146</v>
       </c>
@@ -3919,8 +3920,9 @@
       <c r="O6" s="13" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="P6" s="27"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>146</v>
       </c>
@@ -3958,8 +3960,9 @@
       <c r="O7" s="13" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7" s="27"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>146</v>
       </c>
@@ -4001,8 +4004,9 @@
       <c r="O8" s="13" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8" s="27"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>146</v>
       </c>
@@ -4044,8 +4048,9 @@
       <c r="O9" s="13" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9" s="27"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -4078,7 +4083,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>146</v>
       </c>
@@ -4124,8 +4129,9 @@
       <c r="O11" s="14" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="77.5">
+      <c r="P11" s="27"/>
+    </row>
+    <row r="12" spans="1:16" ht="78" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>146</v>
       </c>
@@ -4161,8 +4167,9 @@
       <c r="O12" s="15" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="P12" s="27"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>146</v>
       </c>
@@ -4200,8 +4207,9 @@
       <c r="O13" s="14" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13" s="27"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>146</v>
       </c>
@@ -4243,8 +4251,9 @@
       <c r="O14" s="14" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14" s="27"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>146</v>
       </c>
@@ -4286,8 +4295,9 @@
       <c r="O15" s="14" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="P15" s="27"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>146</v>
       </c>
@@ -4329,8 +4339,9 @@
       <c r="O16" s="14" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="P16" s="27"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -4363,7 +4374,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="62">
+    <row r="18" spans="1:16" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -4399,8 +4410,9 @@
       <c r="O18" s="16" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="P18" s="27"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>146</v>
       </c>
@@ -4442,8 +4454,9 @@
       <c r="O19" s="13" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="P19" s="27"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>146</v>
       </c>
@@ -4485,8 +4498,9 @@
       <c r="O20" s="13" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" ht="46.5">
+      <c r="P20" s="27"/>
+    </row>
+    <row r="21" spans="1:16" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -4520,8 +4534,9 @@
       <c r="O21" s="15" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="P21" s="27"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>146</v>
       </c>
@@ -4563,8 +4578,9 @@
       <c r="O22" s="14" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="P22" s="27"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -4596,8 +4612,9 @@
       <c r="O23" s="17" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" ht="62">
+      <c r="P23" s="27"/>
+    </row>
+    <row r="24" spans="1:16" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>146</v>
       </c>
@@ -4642,7 +4659,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>146</v>
       </c>
@@ -4685,7 +4702,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>146</v>
       </c>
@@ -4728,7 +4745,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>146</v>
       </c>
@@ -4771,7 +4788,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>146</v>
       </c>
@@ -4814,7 +4831,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>146</v>
       </c>
@@ -4857,7 +4874,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -4890,7 +4907,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="62">
+    <row r="31" spans="1:16" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>146</v>
       </c>
@@ -4935,7 +4952,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>146</v>
       </c>
@@ -4978,7 +4995,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>146</v>
       </c>
@@ -5017,7 +5034,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>146</v>
       </c>
@@ -5056,7 +5073,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -5089,7 +5106,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="62">
+    <row r="36" spans="1:15" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>146</v>
       </c>
@@ -5136,7 +5153,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>146</v>
       </c>
@@ -5179,7 +5196,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>146</v>
       </c>
@@ -5222,7 +5239,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -5255,7 +5272,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>146</v>
       </c>
@@ -5298,7 +5315,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>146</v>
       </c>
@@ -5341,7 +5358,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>146</v>
       </c>
@@ -5380,7 +5397,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>146</v>
       </c>
@@ -5419,7 +5436,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>146</v>
       </c>
@@ -5458,7 +5475,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>146</v>
       </c>
@@ -5497,7 +5514,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -5530,7 +5547,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="62">
+    <row r="47" spans="1:15" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>146</v>
       </c>
@@ -5577,7 +5594,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>146</v>
       </c>
@@ -5616,7 +5633,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>146</v>
       </c>
@@ -5657,7 +5674,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>146</v>
       </c>
@@ -5702,7 +5719,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>146</v>
       </c>
@@ -5745,7 +5762,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -5778,7 +5795,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="62">
+    <row r="53" spans="1:15" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>146</v>
       </c>
@@ -5825,7 +5842,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>146</v>
       </c>
@@ -5866,7 +5883,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>146</v>
       </c>
@@ -5907,7 +5924,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>146</v>
       </c>
@@ -5946,7 +5963,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>146</v>
       </c>
@@ -5987,7 +6004,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>146</v>
       </c>
@@ -6026,7 +6043,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>146</v>
       </c>
@@ -6065,7 +6082,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>146</v>
       </c>
@@ -6110,7 +6127,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>146</v>
       </c>
@@ -6153,7 +6170,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
@@ -6186,7 +6203,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>146</v>
       </c>
@@ -6231,7 +6248,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="62">
+    <row r="64" spans="1:15" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>146</v>
       </c>
@@ -6274,7 +6291,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="62">
+    <row r="65" spans="1:15" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>146</v>
       </c>
@@ -6319,7 +6336,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>146</v>
       </c>
@@ -6362,7 +6379,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>146</v>
       </c>
@@ -6405,7 +6422,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>146</v>
       </c>
@@ -6448,7 +6465,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>146</v>
       </c>
@@ -6487,7 +6504,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>146</v>
       </c>
@@ -6526,7 +6543,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>146</v>
       </c>
@@ -6565,7 +6582,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>146</v>
       </c>
@@ -6604,7 +6621,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>146</v>
       </c>
@@ -6643,7 +6660,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>146</v>
       </c>
@@ -6682,7 +6699,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>146</v>
       </c>
@@ -6721,7 +6738,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
@@ -6754,7 +6771,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>146</v>
       </c>
@@ -6799,7 +6816,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>146</v>
       </c>
@@ -6844,7 +6861,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>146</v>
       </c>
@@ -6887,7 +6904,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>146</v>
       </c>
@@ -6930,7 +6947,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>146</v>
       </c>
@@ -6973,7 +6990,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>146</v>
       </c>
@@ -7016,7 +7033,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="62">
+    <row r="83" spans="1:15" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>146</v>
       </c>
@@ -7059,7 +7076,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -7092,7 +7109,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="62">
+    <row r="85" spans="1:15" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
@@ -7129,7 +7146,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>146</v>
       </c>
@@ -7172,7 +7189,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="87" spans="1:15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>146</v>
       </c>
@@ -7211,7 +7228,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="88" spans="1:15">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>146</v>
       </c>
@@ -7250,7 +7267,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="89" spans="1:15">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>146</v>
       </c>
@@ -7293,7 +7310,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="90" spans="1:15">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>146</v>
       </c>
@@ -7336,7 +7353,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" s="5"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
@@ -7369,7 +7386,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="92" spans="1:15">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" s="4"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -7402,7 +7419,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="93" spans="1:15">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" s="4"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -7439,7 +7456,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="94" spans="1:15">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" s="4"/>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -7472,7 +7489,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="95" spans="1:15">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" s="4"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -7503,7 +7520,7 @@
       </c>
       <c r="O95" s="13"/>
     </row>
-    <row r="96" spans="1:15">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" s="4"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -7532,7 +7549,7 @@
       </c>
       <c r="O96" s="13"/>
     </row>
-    <row r="97" spans="1:15">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" s="4"/>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -7565,7 +7582,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="98" spans="1:15">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" s="5"/>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
@@ -7602,7 +7619,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="99" spans="1:15">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
@@ -7633,7 +7650,7 @@
       </c>
       <c r="O99" s="14"/>
     </row>
-    <row r="100" spans="1:15">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" s="5"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
@@ -7662,7 +7679,7 @@
       </c>
       <c r="O100" s="14"/>
     </row>
-    <row r="101" spans="1:15">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" s="5"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>

</xml_diff>

<commit_message>
modif du mapping, corrections erreurs
</commit_message>
<xml_diff>
--- a/Data Hospital/Hopital Mapping VF.xlsx
+++ b/Data Hospital/Hopital Mapping VF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\Documents\ETUDE\UTC semestre 4\NF26\Smart-Teem\nf26_smart_teem\Data Hospital\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F3C96F-77FE-47A6-87F8-26347C8BBFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9198F1A5-1236-41D5-BDE4-38DC237B1B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="-16200" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{783B3F39-6BFD-C940-8606-2E6B97310E4C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{783B3F39-6BFD-C940-8606-2E6B97310E4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Staging" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1771" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1771" uniqueCount="313">
   <si>
     <t>PK</t>
   </si>
@@ -981,6 +981,12 @@
   <si>
     <t>Surrogate Key : Séquence incrémentale selon les valeurs uniques de la combinaison ID_PATIENT, 'Patient'.
 Il ne faut pas utiliser la fonction automatique IDENTITY.</t>
+  </si>
+  <si>
+    <t>ID_CONSULT_HOSPI</t>
+  </si>
+  <si>
+    <t>NO_CHAMBRE_HOPSI</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1022,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1050,6 +1056,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1156,7 +1168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1185,6 +1197,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1206,7 +1219,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1573,20 +1586,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -3662,9 +3675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAFCA74-9FC5-C241-99E0-C2C69841C5BE}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K86" sqref="K86"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O99" sqref="O99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3683,25 +3696,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="24" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="27"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -3796,7 +3809,7 @@
       <c r="O3" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P3" s="27"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -3840,7 +3853,7 @@
       <c r="O4" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P4" s="27"/>
+      <c r="P4" s="28"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -3880,7 +3893,7 @@
       <c r="O5" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P5" s="27"/>
+      <c r="P5" s="28"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -3920,7 +3933,7 @@
       <c r="O6" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P6" s="27"/>
+      <c r="P6" s="28"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -3960,7 +3973,7 @@
       <c r="O7" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P7" s="27"/>
+      <c r="P7" s="28"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -4004,7 +4017,7 @@
       <c r="O8" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P8" s="27"/>
+      <c r="P8" s="28"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
@@ -4048,7 +4061,7 @@
       <c r="O9" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P9" s="27"/>
+      <c r="P9" s="28"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -4082,6 +4095,7 @@
       <c r="O10" s="13" t="s">
         <v>274</v>
       </c>
+      <c r="P10" s="20"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
@@ -4129,7 +4143,7 @@
       <c r="O11" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P11" s="27"/>
+      <c r="P11" s="20"/>
     </row>
     <row r="12" spans="1:16" ht="78" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
@@ -4167,7 +4181,7 @@
       <c r="O12" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="P12" s="27"/>
+      <c r="P12" s="20"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
@@ -4207,7 +4221,7 @@
       <c r="O13" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P13" s="27"/>
+      <c r="P13" s="20"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
@@ -4251,7 +4265,7 @@
       <c r="O14" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P14" s="27"/>
+      <c r="P14" s="20"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
@@ -4295,7 +4309,7 @@
       <c r="O15" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P15" s="27"/>
+      <c r="P15" s="20"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
@@ -4339,7 +4353,7 @@
       <c r="O16" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P16" s="27"/>
+      <c r="P16" s="20"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
@@ -4373,6 +4387,7 @@
       <c r="O17" s="14" t="s">
         <v>274</v>
       </c>
+      <c r="P17" s="20"/>
     </row>
     <row r="18" spans="1:16" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
@@ -4410,7 +4425,7 @@
       <c r="O18" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="P18" s="27"/>
+      <c r="P18" s="20"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
@@ -4454,7 +4469,7 @@
       <c r="O19" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P19" s="27"/>
+      <c r="P19" s="20"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
@@ -4498,7 +4513,7 @@
       <c r="O20" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P20" s="27"/>
+      <c r="P20" s="20"/>
     </row>
     <row r="21" spans="1:16" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
@@ -4534,7 +4549,7 @@
       <c r="O21" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="P21" s="27"/>
+      <c r="P21" s="20"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
@@ -4578,7 +4593,7 @@
       <c r="O22" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P22" s="27"/>
+      <c r="P22" s="20"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
@@ -4612,7 +4627,7 @@
       <c r="O23" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="P23" s="27"/>
+      <c r="P23" s="20"/>
     </row>
     <row r="24" spans="1:16" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
@@ -4658,7 +4673,7 @@
       <c r="O24" s="16" t="s">
         <v>277</v>
       </c>
-      <c r="P24" s="27"/>
+      <c r="P24" s="20"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
@@ -4702,7 +4717,7 @@
       <c r="O25" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P25" s="27"/>
+      <c r="P25" s="20"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
@@ -4746,7 +4761,7 @@
       <c r="O26" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P26" s="27"/>
+      <c r="P26" s="20"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
@@ -4790,7 +4805,7 @@
       <c r="O27" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P27" s="27"/>
+      <c r="P27" s="20"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
@@ -4834,7 +4849,7 @@
       <c r="O28" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P28" s="27"/>
+      <c r="P28" s="20"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
@@ -4878,7 +4893,7 @@
       <c r="O29" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P29" s="27"/>
+      <c r="P29" s="20"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
@@ -4912,6 +4927,7 @@
       <c r="O30" s="13" t="s">
         <v>274</v>
       </c>
+      <c r="P30" s="20"/>
     </row>
     <row r="31" spans="1:16" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
@@ -4957,7 +4973,7 @@
       <c r="O31" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="P31" s="27"/>
+      <c r="P31" s="20"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
@@ -5001,7 +5017,7 @@
       <c r="O32" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P32" s="27"/>
+      <c r="P32" s="20"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
@@ -5041,7 +5057,7 @@
       <c r="O33" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P33" s="27"/>
+      <c r="P33" s="20"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
@@ -5081,7 +5097,7 @@
       <c r="O34" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P34" s="27"/>
+      <c r="P34" s="20"/>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
@@ -5115,6 +5131,7 @@
       <c r="O35" s="14" t="s">
         <v>274</v>
       </c>
+      <c r="P35" s="20"/>
     </row>
     <row r="36" spans="1:16" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
@@ -5162,7 +5179,7 @@
       <c r="O36" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="P36" s="27"/>
+      <c r="P36" s="20"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
@@ -5206,7 +5223,7 @@
       <c r="O37" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P37" s="27"/>
+      <c r="P37" s="20"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
@@ -5250,7 +5267,7 @@
       <c r="O38" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P38" s="27"/>
+      <c r="P38" s="20"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
@@ -5284,6 +5301,7 @@
       <c r="O39" s="18" t="s">
         <v>272</v>
       </c>
+      <c r="P39" s="20"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
@@ -5327,7 +5345,7 @@
       <c r="O40" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P40" s="27"/>
+      <c r="P40" s="20"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
@@ -5371,7 +5389,7 @@
       <c r="O41" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P41" s="27"/>
+      <c r="P41" s="20"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
@@ -5411,7 +5429,7 @@
       <c r="O42" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P42" s="27"/>
+      <c r="P42" s="20"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
@@ -5451,7 +5469,7 @@
       <c r="O43" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P43" s="27"/>
+      <c r="P43" s="20"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
@@ -5491,7 +5509,7 @@
       <c r="O44" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P44" s="27"/>
+      <c r="P44" s="20"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
@@ -5531,7 +5549,7 @@
       <c r="O45" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P45" s="27"/>
+      <c r="P45" s="20"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="4"/>
@@ -5565,6 +5583,7 @@
       <c r="O46" s="13" t="s">
         <v>274</v>
       </c>
+      <c r="P46" s="20"/>
     </row>
     <row r="47" spans="1:16" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
@@ -5612,7 +5631,7 @@
       <c r="O47" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="P47" s="27"/>
+      <c r="P47" s="20"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
@@ -5652,7 +5671,7 @@
       <c r="O48" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P48" s="27"/>
+      <c r="P48" s="20"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
@@ -5694,7 +5713,7 @@
       <c r="O49" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P49" s="27"/>
+      <c r="P49" s="20"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
@@ -5740,7 +5759,7 @@
       <c r="O50" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P50" s="27"/>
+      <c r="P50" s="20"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
@@ -5784,7 +5803,7 @@
       <c r="O51" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P51" s="27"/>
+      <c r="P51" s="20"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
@@ -5818,6 +5837,7 @@
       <c r="O52" s="14" t="s">
         <v>274</v>
       </c>
+      <c r="P52" s="20"/>
     </row>
     <row r="53" spans="1:16" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
@@ -5865,7 +5885,7 @@
       <c r="O53" s="16" t="s">
         <v>278</v>
       </c>
-      <c r="P53" s="27"/>
+      <c r="P53" s="20"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
@@ -5907,7 +5927,7 @@
       <c r="O54" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P54" s="27"/>
+      <c r="P54" s="20"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
@@ -5949,7 +5969,7 @@
       <c r="O55" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P55" s="27"/>
+      <c r="P55" s="20"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
@@ -5989,7 +6009,7 @@
       <c r="O56" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P56" s="27"/>
+      <c r="P56" s="20"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
@@ -6031,7 +6051,7 @@
       <c r="O57" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P57" s="27"/>
+      <c r="P57" s="20"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
@@ -6071,7 +6091,7 @@
       <c r="O58" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P58" s="27"/>
+      <c r="P58" s="20"/>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
@@ -6111,7 +6131,7 @@
       <c r="O59" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P59" s="27"/>
+      <c r="P59" s="20"/>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
@@ -6157,7 +6177,7 @@
       <c r="O60" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P60" s="27"/>
+      <c r="P60" s="20"/>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
@@ -6201,7 +6221,7 @@
       <c r="O61" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P61" s="27"/>
+      <c r="P61" s="20"/>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="4"/>
@@ -6235,6 +6255,7 @@
       <c r="O62" s="13" t="s">
         <v>274</v>
       </c>
+      <c r="P62" s="20"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
@@ -6280,7 +6301,7 @@
       <c r="O63" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P63" s="27"/>
+      <c r="P63" s="20"/>
     </row>
     <row r="64" spans="1:16" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
@@ -6324,7 +6345,7 @@
       <c r="O64" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="P64" s="27"/>
+      <c r="P64" s="20"/>
     </row>
     <row r="65" spans="1:16" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
@@ -6370,7 +6391,7 @@
       <c r="O65" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="P65" s="27"/>
+      <c r="P65" s="20"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
@@ -6414,7 +6435,7 @@
       <c r="O66" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P66" s="27"/>
+      <c r="P66" s="20"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
@@ -6458,7 +6479,7 @@
       <c r="O67" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P67" s="27"/>
+      <c r="P67" s="20"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
@@ -6502,7 +6523,7 @@
       <c r="O68" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P68" s="27"/>
+      <c r="P68" s="20"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
@@ -6542,7 +6563,7 @@
       <c r="O69" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P69" s="27"/>
+      <c r="P69" s="20"/>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
@@ -6582,7 +6603,7 @@
       <c r="O70" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P70" s="27"/>
+      <c r="P70" s="20"/>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
@@ -6622,7 +6643,7 @@
       <c r="O71" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P71" s="27"/>
+      <c r="P71" s="20"/>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
@@ -6662,7 +6683,7 @@
       <c r="O72" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P72" s="27"/>
+      <c r="P72" s="20"/>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
@@ -6702,7 +6723,7 @@
       <c r="O73" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="P73" s="27"/>
+      <c r="P73" s="20"/>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
@@ -6742,7 +6763,7 @@
       <c r="O74" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P74" s="27"/>
+      <c r="P74" s="20"/>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
@@ -6782,7 +6803,7 @@
       <c r="O75" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="P75" s="27"/>
+      <c r="P75" s="20"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="5"/>
@@ -6816,6 +6837,7 @@
       <c r="O76" s="14" t="s">
         <v>274</v>
       </c>
+      <c r="P76" s="20"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
@@ -6861,7 +6883,7 @@
       <c r="O77" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P77" s="27"/>
+      <c r="P77" s="20"/>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
@@ -6871,7 +6893,7 @@
         <v>158</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>41</v>
+        <v>311</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>152</v>
@@ -6907,7 +6929,7 @@
       <c r="O78" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P78" s="27"/>
+      <c r="P78" s="20"/>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
@@ -6917,7 +6939,7 @@
         <v>158</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>1</v>
+        <v>312</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>160</v>
@@ -6951,7 +6973,7 @@
       <c r="O79" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P79" s="27"/>
+      <c r="P79" s="20"/>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
@@ -6995,7 +7017,7 @@
       <c r="O80" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P80" s="27"/>
+      <c r="P80" s="20"/>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
@@ -7039,7 +7061,7 @@
       <c r="O81" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P81" s="27"/>
+      <c r="P81" s="20"/>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
@@ -7083,7 +7105,7 @@
       <c r="O82" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="P82" s="27"/>
+      <c r="P82" s="20"/>
     </row>
     <row r="83" spans="1:16" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
@@ -7127,7 +7149,7 @@
       <c r="O83" s="16" t="s">
         <v>280</v>
       </c>
-      <c r="P83" s="27"/>
+      <c r="P83" s="20"/>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="4"/>
@@ -7161,6 +7183,7 @@
       <c r="O84" s="13" t="s">
         <v>274</v>
       </c>
+      <c r="P84" s="20"/>
     </row>
     <row r="85" spans="1:16" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A85" s="5"/>
@@ -7198,7 +7221,7 @@
       <c r="O85" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="P85" s="27"/>
+      <c r="P85" s="20"/>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
@@ -7242,7 +7265,7 @@
       <c r="O86" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P86" s="27"/>
+      <c r="P86" s="20"/>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
@@ -7282,7 +7305,7 @@
       <c r="O87" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P87" s="27"/>
+      <c r="P87" s="20"/>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
@@ -7322,7 +7345,7 @@
       <c r="O88" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P88" s="27"/>
+      <c r="P88" s="20"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
@@ -7366,7 +7389,7 @@
       <c r="O89" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P89" s="27"/>
+      <c r="P89" s="20"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
@@ -7410,7 +7433,7 @@
       <c r="O90" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="P90" s="27"/>
+      <c r="P90" s="20"/>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="5"/>
@@ -7444,6 +7467,7 @@
       <c r="O91" s="14" t="s">
         <v>274</v>
       </c>
+      <c r="P91" s="20"/>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" s="4"/>

</xml_diff>